<commit_message>
add v1.4.1 and ER1.3.4
</commit_message>
<xml_diff>
--- a/xyg/xyg数据库数据字典-王哲峰-20200927-v1.4.xlsx
+++ b/xyg/xyg数据库数据字典-王哲峰-20200927-v1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\data-analysis\xyg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2456AC0B-753A-4CCA-9790-6E869E93F072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934A5CD-3BE1-488B-8538-191E27891171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="988" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11076" yWindow="720" windowWidth="15336" windowHeight="10836" tabRatio="988" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="建表说明-TODO" sheetId="34" r:id="rId1"/>
@@ -3065,39 +3065,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3110,7 +3077,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3119,8 +3098,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3442,7 +3442,7 @@
       <c r="A2" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="74" t="s">
         <v>399</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -3460,12 +3460,12 @@
       <c r="A3" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="68" t="s">
+      <c r="D3" s="75"/>
+      <c r="E3" s="78" t="s">
         <v>456</v>
       </c>
       <c r="F3" s="22"/>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="79" t="s">
         <v>457</v>
       </c>
       <c r="H3" s="31" t="s">
@@ -3476,10 +3476,10 @@
       <c r="A4" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="69"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="72"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="31" t="s">
         <v>459</v>
       </c>
@@ -3488,10 +3488,10 @@
       <c r="A5" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="69"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="67"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="72"/>
+      <c r="G5" s="80"/>
       <c r="H5" s="31" t="s">
         <v>419</v>
       </c>
@@ -3500,12 +3500,12 @@
       <c r="A6" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="66" t="s">
+      <c r="D6" s="75"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="70" t="s">
         <v>452</v>
       </c>
-      <c r="G6" s="66" t="s">
+      <c r="G6" s="70" t="s">
         <v>437</v>
       </c>
       <c r="H6" s="31" t="s">
@@ -3513,19 +3513,19 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="64"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="31" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="64"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66" t="s">
+      <c r="D8" s="75"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70" t="s">
         <v>497</v>
       </c>
       <c r="H8" s="31" t="s">
@@ -3539,10 +3539,10 @@
       <c r="B9" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="31" t="s">
         <v>461</v>
       </c>
@@ -3551,10 +3551,10 @@
       <c r="A10" t="s">
         <v>564</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
       <c r="H10" s="31" t="s">
         <v>426</v>
       </c>
@@ -3563,10 +3563,10 @@
       <c r="A11" t="s">
         <v>563</v>
       </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
       <c r="H11" s="31" t="s">
         <v>462</v>
       </c>
@@ -3575,10 +3575,10 @@
       <c r="A12" t="s">
         <v>565</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="69"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="73" t="s">
+      <c r="G12" s="81" t="s">
         <v>463</v>
       </c>
       <c r="H12" s="31" t="s">
@@ -3590,10 +3590,10 @@
         <v>561</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="69"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="66"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="31" t="s">
         <v>465</v>
       </c>
@@ -3603,10 +3603,10 @@
         <v>567</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="69"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="70" t="s">
         <v>58</v>
       </c>
       <c r="H14" s="31" t="s">
@@ -3618,10 +3618,10 @@
         <v>566</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="69"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="66"/>
+      <c r="G15" s="70"/>
       <c r="H15" s="31" t="s">
         <v>115</v>
       </c>
@@ -3630,10 +3630,10 @@
       <c r="A16" t="s">
         <v>614</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="69"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="66"/>
+      <c r="G16" s="70"/>
       <c r="H16" s="31" t="s">
         <v>116</v>
       </c>
@@ -3643,10 +3643,10 @@
         <v>613</v>
       </c>
       <c r="B17" s="20"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="69"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="67"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="70" t="s">
         <v>489</v>
       </c>
       <c r="H17" s="31" t="s">
@@ -3654,28 +3654,28 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="64"/>
-      <c r="E18" s="69"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="67"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="66"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="32" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="64"/>
-      <c r="E19" s="69"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="67"/>
       <c r="F19" s="23"/>
-      <c r="G19" s="66"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="31" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="64"/>
-      <c r="E20" s="69"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="67"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="70" t="s">
         <v>491</v>
       </c>
       <c r="H20" s="31" t="s">
@@ -3683,23 +3683,23 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="65"/>
-      <c r="E21" s="70"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="68"/>
       <c r="F21" s="41"/>
-      <c r="G21" s="67"/>
+      <c r="G21" s="71"/>
       <c r="H21" s="34" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="74" t="s">
         <v>400</v>
       </c>
-      <c r="E22" s="81" t="s">
+      <c r="E22" s="77" t="s">
         <v>400</v>
       </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="78" t="s">
+      <c r="G22" s="69" t="s">
         <v>404</v>
       </c>
       <c r="H22" s="30" t="s">
@@ -3707,21 +3707,21 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="64"/>
-      <c r="E23" s="79"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="66"/>
+      <c r="G23" s="70"/>
       <c r="H23" s="31" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="64"/>
-      <c r="E24" s="79" t="s">
+      <c r="D24" s="75"/>
+      <c r="E24" s="72" t="s">
         <v>407</v>
       </c>
       <c r="F24" s="24"/>
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="70" t="s">
         <v>53</v>
       </c>
       <c r="H24" s="31" t="s">
@@ -3729,100 +3729,100 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="64"/>
-      <c r="E25" s="79"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="66"/>
+      <c r="G25" s="70"/>
       <c r="H25" s="31" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="64"/>
-      <c r="E26" s="79"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="24"/>
-      <c r="G26" s="66"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="31" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="64"/>
-      <c r="E27" s="79"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="66"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="31" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="64"/>
-      <c r="E28" s="79"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="66"/>
+      <c r="G28" s="70"/>
       <c r="H28" s="31" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="64"/>
-      <c r="E29" s="79"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="66"/>
+      <c r="G29" s="70"/>
       <c r="H29" s="31" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="64"/>
-      <c r="E30" s="79"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="72"/>
       <c r="F30" s="24"/>
-      <c r="G30" s="66"/>
+      <c r="G30" s="70"/>
       <c r="H30" s="31" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="64"/>
-      <c r="E31" s="79"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="72"/>
       <c r="F31" s="24"/>
-      <c r="G31" s="66"/>
+      <c r="G31" s="70"/>
       <c r="H31" s="31" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="64"/>
-      <c r="E32" s="79"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="72"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="66"/>
+      <c r="G32" s="70"/>
       <c r="H32" s="31" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" s="64"/>
-      <c r="E33" s="79"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="66"/>
+      <c r="G33" s="70"/>
       <c r="H33" s="31" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="64"/>
-      <c r="E34" s="79"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="72"/>
       <c r="F34" s="24"/>
-      <c r="G34" s="66"/>
+      <c r="G34" s="70"/>
       <c r="H34" s="31" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" s="64"/>
-      <c r="E35" s="79"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="72"/>
       <c r="F35" s="24"/>
-      <c r="G35" s="66" t="s">
+      <c r="G35" s="70" t="s">
         <v>54</v>
       </c>
       <c r="H35" s="31" t="s">
@@ -3830,19 +3830,19 @@
       </c>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" s="64"/>
-      <c r="E36" s="79"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="72"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="66"/>
+      <c r="G36" s="70"/>
       <c r="H36" s="31" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="64"/>
-      <c r="E37" s="79"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="72"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="66" t="s">
+      <c r="G37" s="70" t="s">
         <v>58</v>
       </c>
       <c r="H37" s="31" t="s">
@@ -3850,172 +3850,172 @@
       </c>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="64"/>
-      <c r="E38" s="79"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="24"/>
-      <c r="G38" s="66"/>
+      <c r="G38" s="70"/>
       <c r="H38" s="31" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="64"/>
-      <c r="E39" s="79"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="66"/>
+      <c r="G39" s="70"/>
       <c r="H39" s="31" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="64"/>
-      <c r="E40" s="79"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="72"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="66"/>
+      <c r="G40" s="70"/>
       <c r="H40" s="31" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D41" s="64"/>
-      <c r="E41" s="79"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="66"/>
+      <c r="G41" s="70"/>
       <c r="H41" s="31" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="64"/>
-      <c r="E42" s="79"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="24"/>
-      <c r="G42" s="66"/>
+      <c r="G42" s="70"/>
       <c r="H42" s="31" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D43" s="64"/>
-      <c r="E43" s="79"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="24"/>
-      <c r="G43" s="66"/>
+      <c r="G43" s="70"/>
       <c r="H43" s="31" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="44" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D44" s="64"/>
-      <c r="E44" s="79"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="24"/>
-      <c r="G44" s="66"/>
+      <c r="G44" s="70"/>
       <c r="H44" s="31" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D45" s="64"/>
-      <c r="E45" s="79"/>
+      <c r="D45" s="75"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="66"/>
+      <c r="G45" s="70"/>
       <c r="H45" s="31" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D46" s="64"/>
-      <c r="E46" s="79"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="24"/>
-      <c r="G46" s="66"/>
+      <c r="G46" s="70"/>
       <c r="H46" s="31" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="64"/>
-      <c r="E47" s="79"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="66"/>
+      <c r="G47" s="70"/>
       <c r="H47" s="31" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D48" s="64"/>
-      <c r="E48" s="79"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="72"/>
       <c r="F48" s="24"/>
-      <c r="G48" s="66"/>
+      <c r="G48" s="70"/>
       <c r="H48" s="31" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D49" s="64"/>
-      <c r="E49" s="79"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="72"/>
       <c r="F49" s="24"/>
-      <c r="G49" s="66"/>
+      <c r="G49" s="70"/>
       <c r="H49" s="31" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D50" s="64"/>
-      <c r="E50" s="79"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="72"/>
       <c r="F50" s="24"/>
-      <c r="G50" s="66"/>
+      <c r="G50" s="70"/>
       <c r="H50" s="31" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D51" s="64"/>
-      <c r="E51" s="79"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="66"/>
+      <c r="G51" s="70"/>
       <c r="H51" s="31" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D52" s="64"/>
-      <c r="E52" s="79"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="72"/>
       <c r="F52" s="24"/>
-      <c r="G52" s="66"/>
+      <c r="G52" s="70"/>
       <c r="H52" s="31" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D53" s="64"/>
-      <c r="E53" s="79"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="72"/>
       <c r="F53" s="24"/>
-      <c r="G53" s="66"/>
+      <c r="G53" s="70"/>
       <c r="H53" s="31" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="54" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D54" s="64"/>
-      <c r="E54" s="79"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="72"/>
       <c r="F54" s="24"/>
-      <c r="G54" s="66"/>
+      <c r="G54" s="70"/>
       <c r="H54" s="31" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D55" s="64"/>
-      <c r="E55" s="79"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="24"/>
-      <c r="G55" s="66"/>
+      <c r="G55" s="70"/>
       <c r="H55" s="31" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D56" s="64"/>
-      <c r="E56" s="79"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="72"/>
       <c r="F56" s="24"/>
-      <c r="G56" s="66" t="s">
+      <c r="G56" s="70" t="s">
         <v>16</v>
       </c>
       <c r="H56" s="31" t="s">
@@ -4023,57 +4023,57 @@
       </c>
     </row>
     <row r="57" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D57" s="64"/>
-      <c r="E57" s="79"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="72"/>
       <c r="F57" s="24"/>
-      <c r="G57" s="66"/>
+      <c r="G57" s="70"/>
       <c r="H57" s="31" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D58" s="64"/>
-      <c r="E58" s="79"/>
+      <c r="D58" s="75"/>
+      <c r="E58" s="72"/>
       <c r="F58" s="24"/>
-      <c r="G58" s="66"/>
+      <c r="G58" s="70"/>
       <c r="H58" s="31" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="59" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="64"/>
-      <c r="E59" s="79"/>
+      <c r="D59" s="75"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="24"/>
-      <c r="G59" s="66"/>
+      <c r="G59" s="70"/>
       <c r="H59" s="31" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="60" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D60" s="64"/>
-      <c r="E60" s="79"/>
+      <c r="D60" s="75"/>
+      <c r="E60" s="72"/>
       <c r="F60" s="24"/>
-      <c r="G60" s="66"/>
+      <c r="G60" s="70"/>
       <c r="H60" s="31" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="61" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D61" s="64"/>
-      <c r="E61" s="79"/>
+      <c r="D61" s="75"/>
+      <c r="E61" s="72"/>
       <c r="F61" s="24"/>
-      <c r="G61" s="66"/>
+      <c r="G61" s="70"/>
       <c r="H61" s="31" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="62" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D62" s="64"/>
-      <c r="E62" s="79" t="s">
+      <c r="D62" s="75"/>
+      <c r="E62" s="72" t="s">
         <v>406</v>
       </c>
       <c r="F62" s="24"/>
-      <c r="G62" s="66" t="s">
+      <c r="G62" s="70" t="s">
         <v>53</v>
       </c>
       <c r="H62" s="31" t="s">
@@ -4081,19 +4081,19 @@
       </c>
     </row>
     <row r="63" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="64"/>
-      <c r="E63" s="79"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="72"/>
       <c r="F63" s="24"/>
-      <c r="G63" s="66"/>
+      <c r="G63" s="70"/>
       <c r="H63" s="31" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="64" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="64"/>
-      <c r="E64" s="79"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="72"/>
       <c r="F64" s="24"/>
-      <c r="G64" s="66" t="s">
+      <c r="G64" s="70" t="s">
         <v>54</v>
       </c>
       <c r="H64" s="31" t="s">
@@ -4101,19 +4101,19 @@
       </c>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="64"/>
-      <c r="E65" s="79"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="72"/>
       <c r="F65" s="24"/>
-      <c r="G65" s="66"/>
+      <c r="G65" s="70"/>
       <c r="H65" s="35" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="64"/>
-      <c r="E66" s="79"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="72"/>
       <c r="F66" s="24"/>
-      <c r="G66" s="66" t="s">
+      <c r="G66" s="70" t="s">
         <v>58</v>
       </c>
       <c r="H66" s="31" t="s">
@@ -4121,46 +4121,46 @@
       </c>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="64"/>
-      <c r="E67" s="79"/>
+      <c r="D67" s="75"/>
+      <c r="E67" s="72"/>
       <c r="F67" s="24"/>
-      <c r="G67" s="66"/>
+      <c r="G67" s="70"/>
       <c r="H67" s="31" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="64"/>
-      <c r="E68" s="79"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="72"/>
       <c r="F68" s="24"/>
-      <c r="G68" s="66"/>
+      <c r="G68" s="70"/>
       <c r="H68" s="31" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="64"/>
-      <c r="E69" s="79"/>
+      <c r="D69" s="75"/>
+      <c r="E69" s="72"/>
       <c r="F69" s="24"/>
-      <c r="G69" s="66"/>
+      <c r="G69" s="70"/>
       <c r="H69" s="31" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="64"/>
-      <c r="E70" s="79"/>
+      <c r="D70" s="75"/>
+      <c r="E70" s="72"/>
       <c r="F70" s="24"/>
-      <c r="G70" s="66"/>
+      <c r="G70" s="70"/>
       <c r="H70" s="31" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="64"/>
-      <c r="E71" s="79"/>
+      <c r="D71" s="75"/>
+      <c r="E71" s="72"/>
       <c r="F71" s="24"/>
-      <c r="G71" s="66" t="s">
+      <c r="G71" s="70" t="s">
         <v>454</v>
       </c>
       <c r="H71" s="31" t="s">
@@ -4168,48 +4168,48 @@
       </c>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="64"/>
-      <c r="E72" s="79"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="72"/>
       <c r="F72" s="24"/>
-      <c r="G72" s="66"/>
+      <c r="G72" s="70"/>
       <c r="H72" s="31" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="64"/>
-      <c r="E73" s="79"/>
+      <c r="D73" s="75"/>
+      <c r="E73" s="72"/>
       <c r="F73" s="24"/>
-      <c r="G73" s="66"/>
+      <c r="G73" s="70"/>
       <c r="H73" s="31" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="64"/>
-      <c r="E74" s="79"/>
+      <c r="D74" s="75"/>
+      <c r="E74" s="72"/>
       <c r="F74" s="24"/>
-      <c r="G74" s="66"/>
+      <c r="G74" s="70"/>
       <c r="H74" s="39" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="75" spans="4:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="65"/>
-      <c r="E75" s="80"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="73"/>
       <c r="F75" s="33"/>
-      <c r="G75" s="67"/>
+      <c r="G75" s="71"/>
       <c r="H75" s="40" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D76" s="74" t="s">
+      <c r="D76" s="63" t="s">
         <v>401</v>
       </c>
-      <c r="E76" s="77"/>
+      <c r="E76" s="66"/>
       <c r="F76" s="37"/>
-      <c r="G76" s="78" t="s">
+      <c r="G76" s="69" t="s">
         <v>130</v>
       </c>
       <c r="H76" s="30" t="s">
@@ -4217,25 +4217,35 @@
       </c>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D77" s="75"/>
-      <c r="E77" s="69"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="67"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="66"/>
+      <c r="G77" s="70"/>
       <c r="H77" s="35" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="78" spans="4:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="76"/>
-      <c r="E78" s="70"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="68"/>
       <c r="F78" s="41"/>
-      <c r="G78" s="67"/>
+      <c r="G78" s="71"/>
       <c r="H78" s="34" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D2:D21"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="E3:E21"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="D76:D78"/>
     <mergeCell ref="E76:E78"/>
     <mergeCell ref="G76:G78"/>
@@ -4252,16 +4262,6 @@
     <mergeCell ref="G66:G70"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="G35:G36"/>
-    <mergeCell ref="D2:D21"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="E3:E21"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F6:F11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4277,7 +4277,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4918,7 +4918,9 @@
   </sheetPr>
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7969,8 +7971,8 @@
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView view="pageLayout" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8449,6 +8451,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9259,8 +9262,8 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -16173,8 +16176,8 @@
   </sheetPr>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90:E91"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -24134,8 +24137,8 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -29255,8 +29258,8 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:B39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -30417,7 +30420,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -30571,7 +30574,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -30783,7 +30786,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>